<commit_message>
Next step: create product modals
</commit_message>
<xml_diff>
--- a/other files/Working Copy of Alias change STD Products 3-30-21 - Murray.xlsx
+++ b/other files/Working Copy of Alias change STD Products 3-30-21 - Murray.xlsx
@@ -4803,7 +4803,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -20183,12 +20183,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N437"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A225" sqref="A225"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20250,7 +20249,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>611</v>
       </c>
@@ -20288,7 +20287,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>577</v>
       </c>
@@ -20326,7 +20325,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>628</v>
       </c>
@@ -20364,7 +20363,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>576</v>
       </c>
@@ -20402,7 +20401,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>644</v>
       </c>
@@ -20440,7 +20439,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>575</v>
       </c>
@@ -20478,7 +20477,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>661</v>
       </c>
@@ -20516,7 +20515,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>574</v>
       </c>
@@ -20554,7 +20553,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>598</v>
       </c>
@@ -20592,7 +20591,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>573</v>
       </c>
@@ -20627,7 +20626,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>613</v>
       </c>
@@ -20665,7 +20664,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>572</v>
       </c>
@@ -20703,7 +20702,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>629</v>
       </c>
@@ -20741,7 +20740,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>571</v>
       </c>
@@ -20779,7 +20778,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>645</v>
       </c>
@@ -20817,7 +20816,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>570</v>
       </c>
@@ -20855,7 +20854,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>662</v>
       </c>
@@ -20893,7 +20892,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>569</v>
       </c>
@@ -20931,7 +20930,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>599</v>
       </c>
@@ -20969,7 +20968,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>568</v>
       </c>
@@ -21004,7 +21003,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>614</v>
       </c>
@@ -21042,7 +21041,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>567</v>
       </c>
@@ -21080,7 +21079,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>630</v>
       </c>
@@ -21118,7 +21117,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>566</v>
       </c>
@@ -21156,7 +21155,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>646</v>
       </c>
@@ -21194,7 +21193,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>565</v>
       </c>
@@ -21232,7 +21231,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>663</v>
       </c>
@@ -21270,7 +21269,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>564</v>
       </c>
@@ -21308,7 +21307,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>600</v>
       </c>
@@ -21346,7 +21345,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>563</v>
       </c>
@@ -21381,7 +21380,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>616</v>
       </c>
@@ -21419,7 +21418,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>562</v>
       </c>
@@ -21457,7 +21456,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>632</v>
       </c>
@@ -21495,7 +21494,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>525</v>
       </c>
@@ -21533,7 +21532,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>648</v>
       </c>
@@ -21571,7 +21570,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>561</v>
       </c>
@@ -21609,7 +21608,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>664</v>
       </c>
@@ -21647,7 +21646,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>560</v>
       </c>
@@ -21685,7 +21684,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>601</v>
       </c>
@@ -21723,7 +21722,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>559</v>
       </c>
@@ -21758,7 +21757,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>617</v>
       </c>
@@ -21796,7 +21795,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>558</v>
       </c>
@@ -21834,7 +21833,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>633</v>
       </c>
@@ -21872,7 +21871,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>557</v>
       </c>
@@ -21910,7 +21909,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>649</v>
       </c>
@@ -21948,7 +21947,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>556</v>
       </c>
@@ -21986,7 +21985,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>665</v>
       </c>
@@ -22024,7 +22023,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>555</v>
       </c>
@@ -22062,7 +22061,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>602</v>
       </c>
@@ -22100,7 +22099,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>554</v>
       </c>
@@ -22135,7 +22134,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>618</v>
       </c>
@@ -22173,7 +22172,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>553</v>
       </c>
@@ -22211,7 +22210,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>634</v>
       </c>
@@ -22249,7 +22248,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>552</v>
       </c>
@@ -22287,7 +22286,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>650</v>
       </c>
@@ -22325,7 +22324,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>551</v>
       </c>
@@ -22363,7 +22362,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>666</v>
       </c>
@@ -22401,7 +22400,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>550</v>
       </c>
@@ -22439,7 +22438,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>603</v>
       </c>
@@ -22477,7 +22476,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>549</v>
       </c>
@@ -22515,7 +22514,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>620</v>
       </c>
@@ -22553,7 +22552,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>548</v>
       </c>
@@ -22591,7 +22590,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>636</v>
       </c>
@@ -22629,7 +22628,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>547</v>
       </c>
@@ -22667,7 +22666,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>652</v>
       </c>
@@ -22705,7 +22704,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>524</v>
       </c>
@@ -22743,7 +22742,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>667</v>
       </c>
@@ -22781,7 +22780,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>522</v>
       </c>
@@ -22819,7 +22818,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>605</v>
       </c>
@@ -22857,7 +22856,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>521</v>
       </c>
@@ -22892,7 +22891,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>621</v>
       </c>
@@ -22930,7 +22929,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>546</v>
       </c>
@@ -22968,7 +22967,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>637</v>
       </c>
@@ -23006,7 +23005,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>520</v>
       </c>
@@ -23044,7 +23043,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>654</v>
       </c>
@@ -23082,7 +23081,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>545</v>
       </c>
@@ -23120,7 +23119,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>668</v>
       </c>
@@ -23158,7 +23157,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>544</v>
       </c>
@@ -23196,7 +23195,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>606</v>
       </c>
@@ -23234,7 +23233,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>543</v>
       </c>
@@ -23272,7 +23271,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>622</v>
       </c>
@@ -23310,7 +23309,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>518</v>
       </c>
@@ -23348,7 +23347,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>638</v>
       </c>
@@ -23386,7 +23385,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>535</v>
       </c>
@@ -23424,7 +23423,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>655</v>
       </c>
@@ -23462,7 +23461,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>541</v>
       </c>
@@ -23500,7 +23499,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>669</v>
       </c>
@@ -23538,7 +23537,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>539</v>
       </c>
@@ -23576,7 +23575,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>607</v>
       </c>
@@ -23614,7 +23613,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>537</v>
       </c>
@@ -23649,7 +23648,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>624</v>
       </c>
@@ -23687,7 +23686,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>534</v>
       </c>
@@ -23725,7 +23724,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>640</v>
       </c>
@@ -23763,7 +23762,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>533</v>
       </c>
@@ -23801,7 +23800,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>657</v>
       </c>
@@ -23839,7 +23838,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>532</v>
       </c>
@@ -23877,7 +23876,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>671</v>
       </c>
@@ -23915,7 +23914,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>531</v>
       </c>
@@ -23953,7 +23952,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>609</v>
       </c>
@@ -23991,7 +23990,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>471</v>
       </c>
@@ -24026,7 +24025,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>626</v>
       </c>
@@ -24064,7 +24063,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>526</v>
       </c>
@@ -24102,7 +24101,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>642</v>
       </c>
@@ -24140,7 +24139,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>530</v>
       </c>
@@ -24178,7 +24177,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>659</v>
       </c>
@@ -24216,7 +24215,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>529</v>
       </c>
@@ -24254,7 +24253,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>672</v>
       </c>
@@ -24292,7 +24291,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>528</v>
       </c>
@@ -24330,7 +24329,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>610</v>
       </c>
@@ -24368,7 +24367,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>527</v>
       </c>
@@ -24403,7 +24402,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>491</v>
       </c>
@@ -24435,7 +24434,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>485</v>
       </c>
@@ -24467,7 +24466,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>597</v>
       </c>
@@ -24499,7 +24498,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>596</v>
       </c>
@@ -24531,7 +24530,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>496</v>
       </c>
@@ -24563,7 +24562,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>595</v>
       </c>
@@ -24595,7 +24594,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>594</v>
       </c>
@@ -24627,7 +24626,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>593</v>
       </c>
@@ -24659,7 +24658,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>492</v>
       </c>
@@ -24691,7 +24690,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>478</v>
       </c>
@@ -24723,7 +24722,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>476</v>
       </c>
@@ -24755,7 +24754,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>469</v>
       </c>
@@ -24787,7 +24786,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>495</v>
       </c>
@@ -24819,7 +24818,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>484</v>
       </c>
@@ -24851,7 +24850,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>592</v>
       </c>
@@ -24883,7 +24882,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>591</v>
       </c>
@@ -24915,7 +24914,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>493</v>
       </c>
@@ -24947,7 +24946,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>483</v>
       </c>
@@ -24979,7 +24978,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>474</v>
       </c>
@@ -25011,7 +25010,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>590</v>
       </c>
@@ -25043,7 +25042,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>489</v>
       </c>
@@ -25075,7 +25074,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>479</v>
       </c>
@@ -25107,7 +25106,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>473</v>
       </c>
@@ -25139,7 +25138,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="135" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>467</v>
       </c>
@@ -25171,7 +25170,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="136" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>589</v>
       </c>
@@ -25203,7 +25202,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>580</v>
       </c>
@@ -25235,7 +25234,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="138" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>579</v>
       </c>
@@ -25267,7 +25266,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="139" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>578</v>
       </c>
@@ -25299,7 +25298,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="140" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>494</v>
       </c>
@@ -25331,7 +25330,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="141" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>480</v>
       </c>
@@ -25363,7 +25362,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="142" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>477</v>
       </c>
@@ -25395,7 +25394,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>588</v>
       </c>
@@ -25427,7 +25426,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>586</v>
       </c>
@@ -25459,7 +25458,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>486</v>
       </c>
@@ -25491,7 +25490,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>583</v>
       </c>
@@ -25523,7 +25522,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>581</v>
       </c>
@@ -25555,7 +25554,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>490</v>
       </c>
@@ -25587,7 +25586,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>481</v>
       </c>
@@ -25619,7 +25618,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>475</v>
       </c>
@@ -25651,7 +25650,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>470</v>
       </c>
@@ -25683,7 +25682,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>841</v>
       </c>
@@ -25718,7 +25717,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>842</v>
       </c>
@@ -25750,7 +25749,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>1072</v>
       </c>
@@ -25782,7 +25781,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>844</v>
       </c>
@@ -25814,7 +25813,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>845</v>
       </c>
@@ -25846,7 +25845,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>1075</v>
       </c>
@@ -25878,7 +25877,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>846</v>
       </c>
@@ -25910,7 +25909,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>847</v>
       </c>
@@ -25942,7 +25941,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>1078</v>
       </c>
@@ -25974,7 +25973,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>849</v>
       </c>
@@ -26006,7 +26005,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>850</v>
       </c>
@@ -26038,7 +26037,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>1081</v>
       </c>
@@ -26070,7 +26069,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>499</v>
       </c>
@@ -26102,7 +26101,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>851</v>
       </c>
@@ -26134,7 +26133,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>1084</v>
       </c>
@@ -26166,7 +26165,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>1280</v>
       </c>
@@ -26207,7 +26206,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>414</v>
       </c>
@@ -26248,7 +26247,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>852</v>
       </c>
@@ -26289,7 +26288,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A170" s="42" t="s">
         <v>1281</v>
       </c>
@@ -26330,7 +26329,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>413</v>
       </c>
@@ -26371,7 +26370,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>854</v>
       </c>
@@ -26412,7 +26411,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>888</v>
       </c>
@@ -26450,7 +26449,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>887</v>
       </c>
@@ -26488,7 +26487,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>886</v>
       </c>
@@ -26526,7 +26525,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>885</v>
       </c>
@@ -26564,7 +26563,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>884</v>
       </c>
@@ -26602,7 +26601,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>883</v>
       </c>
@@ -26640,7 +26639,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>882</v>
       </c>
@@ -26678,7 +26677,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>881</v>
       </c>
@@ -26716,7 +26715,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="181" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>880</v>
       </c>
@@ -26754,7 +26753,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="182" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>879</v>
       </c>
@@ -26792,7 +26791,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="183" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>878</v>
       </c>
@@ -26830,7 +26829,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="184" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>877</v>
       </c>
@@ -26868,7 +26867,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="185" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>876</v>
       </c>
@@ -26906,7 +26905,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>875</v>
       </c>
@@ -26944,7 +26943,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>855</v>
       </c>
@@ -26982,7 +26981,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>860</v>
       </c>
@@ -27020,7 +27019,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="189" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>856</v>
       </c>
@@ -27058,7 +27057,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>861</v>
       </c>
@@ -27096,7 +27095,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="191" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>412</v>
       </c>
@@ -27134,7 +27133,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="192" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>862</v>
       </c>
@@ -27172,7 +27171,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="193" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>411</v>
       </c>
@@ -27210,7 +27209,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="194" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>863</v>
       </c>
@@ -27248,7 +27247,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="195" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>923</v>
       </c>
@@ -27289,7 +27288,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="196" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>924</v>
       </c>
@@ -27327,7 +27326,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="197" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>925</v>
       </c>
@@ -27365,7 +27364,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="198" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>916</v>
       </c>
@@ -27403,7 +27402,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="199" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>864</v>
       </c>
@@ -27438,7 +27437,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="200" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>488</v>
       </c>
@@ -27473,7 +27472,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="201" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>866</v>
       </c>
@@ -27508,7 +27507,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="202" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>487</v>
       </c>
@@ -27543,7 +27542,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="203" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>498</v>
       </c>
@@ -27581,7 +27580,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="204" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>410</v>
       </c>
@@ -27619,7 +27618,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="205" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>868</v>
       </c>
@@ -27654,7 +27653,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="206" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>409</v>
       </c>
@@ -27689,7 +27688,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="207" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>869</v>
       </c>
@@ -27724,7 +27723,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="208" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>873</v>
       </c>
@@ -27759,7 +27758,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="209" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>870</v>
       </c>
@@ -27794,7 +27793,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="210" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>874</v>
       </c>
@@ -27829,7 +27828,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="211" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>917</v>
       </c>
@@ -27867,7 +27866,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="212" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>914</v>
       </c>
@@ -27905,7 +27904,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="213" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>919</v>
       </c>
@@ -27934,7 +27933,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="214" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>921</v>
       </c>
@@ -27963,7 +27962,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="215" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>912</v>
       </c>
@@ -27992,7 +27991,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="216" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>908</v>
       </c>
@@ -28021,7 +28020,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="217" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>906</v>
       </c>
@@ -28050,7 +28049,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="218" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>910</v>
       </c>
@@ -28079,7 +28078,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="219" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>889</v>
       </c>
@@ -28117,7 +28116,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="220" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>761</v>
       </c>
@@ -28152,7 +28151,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="221" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>780</v>
       </c>
@@ -28190,7 +28189,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="222" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>760</v>
       </c>
@@ -28228,7 +28227,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="223" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>793</v>
       </c>
@@ -28266,7 +28265,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="224" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>437</v>
       </c>
@@ -28304,7 +28303,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>808</v>
       </c>
@@ -28377,7 +28376,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="227" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>762</v>
       </c>
@@ -28415,7 +28414,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="228" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>435</v>
       </c>
@@ -28453,7 +28452,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="229" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>781</v>
       </c>
@@ -28491,7 +28490,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="230" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>759</v>
       </c>
@@ -28529,7 +28528,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="231" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>794</v>
       </c>
@@ -28567,7 +28566,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="232" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>758</v>
       </c>
@@ -28678,7 +28677,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="235" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>764</v>
       </c>
@@ -28716,7 +28715,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="236" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>434</v>
       </c>
@@ -28754,7 +28753,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="237" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>782</v>
       </c>
@@ -28792,7 +28791,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="238" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>433</v>
       </c>
@@ -28830,7 +28829,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="239" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>795</v>
       </c>
@@ -28868,7 +28867,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="240" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>432</v>
       </c>
@@ -28979,7 +28978,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="243" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>766</v>
       </c>
@@ -29017,7 +29016,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="244" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>756</v>
       </c>
@@ -29055,7 +29054,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="245" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>783</v>
       </c>
@@ -29093,7 +29092,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="246" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>755</v>
       </c>
@@ -29131,7 +29130,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="247" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>796</v>
       </c>
@@ -29169,7 +29168,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="248" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>754</v>
       </c>
@@ -29280,7 +29279,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="251" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>767</v>
       </c>
@@ -29318,7 +29317,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="252" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>430</v>
       </c>
@@ -29356,7 +29355,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="253" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>784</v>
       </c>
@@ -29394,7 +29393,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="254" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>752</v>
       </c>
@@ -29432,7 +29431,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="255" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>797</v>
       </c>
@@ -29470,7 +29469,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="256" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>751</v>
       </c>
@@ -29581,7 +29580,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="259" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>769</v>
       </c>
@@ -29619,7 +29618,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="260" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>428</v>
       </c>
@@ -29657,7 +29656,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="261" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>785</v>
       </c>
@@ -29695,7 +29694,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="262" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>750</v>
       </c>
@@ -29733,7 +29732,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="263" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>798</v>
       </c>
@@ -29771,7 +29770,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="264" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>427</v>
       </c>
@@ -29882,7 +29881,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="267" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>771</v>
       </c>
@@ -29920,7 +29919,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="268" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>749</v>
       </c>
@@ -29958,7 +29957,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="269" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>787</v>
       </c>
@@ -29996,7 +29995,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="270" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>748</v>
       </c>
@@ -30034,7 +30033,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="271" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>800</v>
       </c>
@@ -30072,7 +30071,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="272" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>747</v>
       </c>
@@ -30183,7 +30182,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="275" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>772</v>
       </c>
@@ -30221,7 +30220,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="276" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>745</v>
       </c>
@@ -30259,7 +30258,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="277" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>788</v>
       </c>
@@ -30297,7 +30296,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="278" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>744</v>
       </c>
@@ -30335,7 +30334,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="279" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>801</v>
       </c>
@@ -30373,7 +30372,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="280" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>743</v>
       </c>
@@ -30484,7 +30483,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="283" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>773</v>
       </c>
@@ -30522,7 +30521,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="284" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>424</v>
       </c>
@@ -30560,7 +30559,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="285" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>789</v>
       </c>
@@ -30598,7 +30597,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="286" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>738</v>
       </c>
@@ -30636,7 +30635,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="287" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>802</v>
       </c>
@@ -30674,7 +30673,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="288" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>736</v>
       </c>
@@ -30785,7 +30784,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="291" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>775</v>
       </c>
@@ -30823,7 +30822,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="292" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>423</v>
       </c>
@@ -30861,7 +30860,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="293" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>791</v>
       </c>
@@ -30899,7 +30898,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="294" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>735</v>
       </c>
@@ -30937,7 +30936,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="295" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>804</v>
       </c>
@@ -30975,7 +30974,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="296" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>734</v>
       </c>
@@ -31086,7 +31085,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="299" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>777</v>
       </c>
@@ -31124,7 +31123,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="300" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>421</v>
       </c>
@@ -31162,7 +31161,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="301" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>792</v>
       </c>
@@ -31200,7 +31199,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="302" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>420</v>
       </c>
@@ -31238,7 +31237,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="303" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>806</v>
       </c>
@@ -31276,7 +31275,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="304" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>419</v>
       </c>
@@ -31381,7 +31380,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="307" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>417</v>
       </c>
@@ -31410,7 +31409,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="308" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>840</v>
       </c>
@@ -31439,7 +31438,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="309" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>839</v>
       </c>
@@ -31468,7 +31467,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="310" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>838</v>
       </c>
@@ -31497,7 +31496,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="311" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>837</v>
       </c>
@@ -31526,7 +31525,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="312" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>836</v>
       </c>
@@ -31555,7 +31554,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="313" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>835</v>
       </c>
@@ -31584,7 +31583,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="314" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>834</v>
       </c>
@@ -31613,7 +31612,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="315" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>416</v>
       </c>
@@ -31642,7 +31641,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="316" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>833</v>
       </c>
@@ -31671,7 +31670,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="317" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>832</v>
       </c>
@@ -31700,7 +31699,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="318" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>831</v>
       </c>
@@ -31729,7 +31728,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="319" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>415</v>
       </c>
@@ -31758,7 +31757,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="320" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>830</v>
       </c>
@@ -31787,7 +31786,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="321" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>829</v>
       </c>
@@ -31816,7 +31815,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="322" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>828</v>
       </c>
@@ -31845,7 +31844,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="323" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>827</v>
       </c>
@@ -31874,7 +31873,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="324" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>826</v>
       </c>
@@ -31903,7 +31902,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="325" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>825</v>
       </c>
@@ -31932,7 +31931,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="326" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>824</v>
       </c>
@@ -31961,7 +31960,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="327" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>459</v>
       </c>
@@ -31999,7 +31998,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="328" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>701</v>
       </c>
@@ -32037,7 +32036,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="329" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>458</v>
       </c>
@@ -32075,7 +32074,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="330" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>692</v>
       </c>
@@ -32113,7 +32112,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="331" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>722</v>
       </c>
@@ -32151,7 +32150,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="332" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>711</v>
       </c>
@@ -32189,7 +32188,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="333" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>457</v>
       </c>
@@ -32227,7 +32226,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="334" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>702</v>
       </c>
@@ -32265,7 +32264,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="335" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>682</v>
       </c>
@@ -32303,7 +32302,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="336" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>456</v>
       </c>
@@ -32341,7 +32340,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="337" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>723</v>
       </c>
@@ -32379,7 +32378,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="338" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>712</v>
       </c>
@@ -32417,7 +32416,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="339" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>455</v>
       </c>
@@ -32455,7 +32454,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="340" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>454</v>
       </c>
@@ -32493,7 +32492,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="341" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>453</v>
       </c>
@@ -32531,7 +32530,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="342" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>693</v>
       </c>
@@ -32569,7 +32568,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="343" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>724</v>
       </c>
@@ -32607,7 +32606,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="344" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>713</v>
       </c>
@@ -32645,7 +32644,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="345" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>674</v>
       </c>
@@ -32683,7 +32682,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="346" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>704</v>
       </c>
@@ -32721,7 +32720,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="347" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>684</v>
       </c>
@@ -32759,7 +32758,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="348" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>694</v>
       </c>
@@ -32797,7 +32796,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="349" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>725</v>
       </c>
@@ -32835,7 +32834,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="350" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>714</v>
       </c>
@@ -32873,7 +32872,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="351" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>452</v>
       </c>
@@ -32911,7 +32910,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="352" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>451</v>
       </c>
@@ -32949,7 +32948,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="353" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>450</v>
       </c>
@@ -32987,7 +32986,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="354" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>449</v>
       </c>
@@ -33025,7 +33024,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="355" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>726</v>
       </c>
@@ -33063,7 +33062,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="356" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>715</v>
       </c>
@@ -33101,7 +33100,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="357" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>448</v>
       </c>
@@ -33139,7 +33138,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="358" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>447</v>
       </c>
@@ -33177,7 +33176,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="359" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>446</v>
       </c>
@@ -33215,7 +33214,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="360" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>445</v>
       </c>
@@ -33253,7 +33252,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="361" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>727</v>
       </c>
@@ -33291,7 +33290,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="362" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>716</v>
       </c>
@@ -33329,7 +33328,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="363" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>677</v>
       </c>
@@ -33367,7 +33366,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="364" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>707</v>
       </c>
@@ -33405,7 +33404,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="365" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>686</v>
       </c>
@@ -33443,7 +33442,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="366" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>444</v>
       </c>
@@ -33481,7 +33480,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="367" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>728</v>
       </c>
@@ -33519,7 +33518,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="368" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>717</v>
       </c>
@@ -33557,7 +33556,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="369" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>678</v>
       </c>
@@ -33595,7 +33594,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="370" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>708</v>
       </c>
@@ -33633,7 +33632,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="371" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>687</v>
       </c>
@@ -33671,7 +33670,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="372" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>696</v>
       </c>
@@ -33709,7 +33708,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="373" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>729</v>
       </c>
@@ -33747,7 +33746,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="374" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>718</v>
       </c>
@@ -33785,7 +33784,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="375" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>679</v>
       </c>
@@ -33823,7 +33822,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="376" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>443</v>
       </c>
@@ -33861,7 +33860,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="377" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>688</v>
       </c>
@@ -33899,7 +33898,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="378" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>697</v>
       </c>
@@ -33937,7 +33936,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="379" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>730</v>
       </c>
@@ -33975,7 +33974,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="380" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>719</v>
       </c>
@@ -34013,7 +34012,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="381" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>442</v>
       </c>
@@ -34051,7 +34050,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="382" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>441</v>
       </c>
@@ -34089,7 +34088,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="383" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>690</v>
       </c>
@@ -34127,7 +34126,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="384" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>699</v>
       </c>
@@ -34165,7 +34164,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="385" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>732</v>
       </c>
@@ -34203,7 +34202,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="386" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>440</v>
       </c>
@@ -34241,7 +34240,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="387" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>439</v>
       </c>
@@ -34279,7 +34278,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="388" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>438</v>
       </c>
@@ -34317,7 +34316,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="389" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>691</v>
       </c>
@@ -34355,7 +34354,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="390" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>700</v>
       </c>
@@ -34393,7 +34392,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="391" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>733</v>
       </c>
@@ -34431,7 +34430,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="392" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>721</v>
       </c>
@@ -34469,7 +34468,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="393" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>497</v>
       </c>
@@ -34501,7 +34500,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="394" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>482</v>
       </c>
@@ -34533,7 +34532,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="395" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>472</v>
       </c>
@@ -34565,7 +34564,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="396" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>468</v>
       </c>
@@ -34597,7 +34596,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="397" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B397" s="18" t="s">
         <v>1355</v>
       </c>
@@ -34626,7 +34625,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="398" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B398" s="43" t="s">
         <v>1355</v>
       </c>
@@ -34655,7 +34654,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="399" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B399" s="43" t="s">
         <v>1355</v>
       </c>
@@ -34684,7 +34683,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="400" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B400" s="43" t="s">
         <v>1355</v>
       </c>
@@ -34713,7 +34712,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="401" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B401" s="43" t="s">
         <v>1355</v>
       </c>
@@ -34742,7 +34741,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="402" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B402" s="43" t="s">
         <v>1355</v>
       </c>
@@ -34771,7 +34770,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="403" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B403" s="43" t="s">
         <v>1355</v>
       </c>
@@ -34797,7 +34796,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="404" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B404" s="43" t="s">
         <v>1355</v>
       </c>
@@ -34826,7 +34825,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="405" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B405" s="43" t="s">
         <v>1355</v>
       </c>
@@ -34858,7 +34857,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="406" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B406" s="43" t="s">
         <v>1355</v>
       </c>
@@ -34890,7 +34889,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="407" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B407" s="43" t="s">
         <v>1355</v>
       </c>
@@ -34922,7 +34921,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="408" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B408" s="43" t="s">
         <v>1355</v>
       </c>
@@ -34954,7 +34953,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="409" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B409" s="43" t="s">
         <v>1355</v>
       </c>
@@ -34986,7 +34985,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="410" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B410" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35018,7 +35017,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="411" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B411" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35050,7 +35049,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="412" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B412" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35082,7 +35081,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="413" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B413" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35108,7 +35107,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="414" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B414" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35137,7 +35136,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="415" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B415" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35166,7 +35165,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="416" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B416" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35195,7 +35194,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="417" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B417" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35224,7 +35223,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="418" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B418" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35256,7 +35255,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="419" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B419" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35288,7 +35287,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="420" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B420" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35320,7 +35319,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="421" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B421" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35352,7 +35351,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="422" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>1354</v>
       </c>
@@ -35384,7 +35383,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="423" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>1354</v>
       </c>
@@ -35416,7 +35415,7 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="424" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>1354</v>
       </c>
@@ -35448,7 +35447,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="425" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>1354</v>
       </c>
@@ -35480,7 +35479,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="426" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>1354</v>
       </c>
@@ -35512,7 +35511,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="427" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>1354</v>
       </c>
@@ -35544,7 +35543,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="428" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>1354</v>
       </c>
@@ -35573,7 +35572,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="429" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>1354</v>
       </c>
@@ -35605,7 +35604,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="430" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>1354</v>
       </c>
@@ -35637,7 +35636,7 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="431" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>1354</v>
       </c>
@@ -35669,7 +35668,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="432" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>1354</v>
       </c>
@@ -35701,7 +35700,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="433" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>1354</v>
       </c>
@@ -35733,7 +35732,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="434" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>1354</v>
       </c>
@@ -35765,7 +35764,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="435" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>1354</v>
       </c>
@@ -35797,7 +35796,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="436" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>1354</v>
       </c>
@@ -35826,7 +35825,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="437" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>1354</v>
       </c>
@@ -35859,18 +35858,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N437">
-    <filterColumn colId="0">
-      <customFilters>
-        <customFilter val="*IBW*"/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="201-00"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N437"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -36174,18 +36162,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36208,6 +36196,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56C8FBF-B3B9-432D-A40E-5376C0AE01AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02A70B78-95E3-4533-A5C0-CF911D481E23}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="42bcbbcd-ff49-4650-acba-18717079aec5"/>
@@ -36222,12 +36218,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56C8FBF-B3B9-432D-A40E-5376C0AE01AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added loosefill/custom btns more modal work
</commit_message>
<xml_diff>
--- a/other files/Working Copy of Alias change STD Products 3-30-21 - Murray.xlsx
+++ b/other files/Working Copy of Alias change STD Products 3-30-21 - Murray.xlsx
@@ -4803,7 +4803,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -20188,7 +20188,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20478,7 +20478,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>661</v>
       </c>
@@ -20516,7 +20516,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>574</v>
       </c>
@@ -20554,7 +20554,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>598</v>
       </c>
@@ -20592,7 +20592,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>573</v>
       </c>
@@ -20855,7 +20855,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>662</v>
       </c>
@@ -20893,7 +20893,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>569</v>
       </c>
@@ -20931,7 +20931,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>599</v>
       </c>
@@ -20969,7 +20969,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>568</v>
       </c>
@@ -21232,7 +21232,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>663</v>
       </c>
@@ -21270,7 +21270,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>564</v>
       </c>
@@ -21308,7 +21308,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>600</v>
       </c>
@@ -21346,7 +21346,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>563</v>
       </c>
@@ -21609,7 +21609,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>664</v>
       </c>
@@ -21647,7 +21647,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>560</v>
       </c>
@@ -21685,7 +21685,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>601</v>
       </c>
@@ -21723,7 +21723,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>559</v>
       </c>
@@ -21986,7 +21986,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>665</v>
       </c>
@@ -22024,7 +22024,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>555</v>
       </c>
@@ -22062,7 +22062,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>602</v>
       </c>
@@ -22100,7 +22100,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>554</v>
       </c>
@@ -22363,7 +22363,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>666</v>
       </c>
@@ -22401,7 +22401,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>550</v>
       </c>
@@ -22439,7 +22439,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>603</v>
       </c>
@@ -22477,7 +22477,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>549</v>
       </c>
@@ -22743,7 +22743,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>667</v>
       </c>
@@ -22781,7 +22781,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>522</v>
       </c>
@@ -22819,7 +22819,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>605</v>
       </c>
@@ -22857,7 +22857,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>521</v>
       </c>
@@ -23120,7 +23120,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>668</v>
       </c>
@@ -23158,7 +23158,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>544</v>
       </c>
@@ -23196,7 +23196,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>606</v>
       </c>
@@ -23234,7 +23234,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>543</v>
       </c>
@@ -23500,7 +23500,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>669</v>
       </c>
@@ -23538,7 +23538,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>539</v>
       </c>
@@ -23576,7 +23576,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>607</v>
       </c>
@@ -23614,7 +23614,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>537</v>
       </c>
@@ -23877,7 +23877,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>671</v>
       </c>
@@ -23915,7 +23915,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>531</v>
       </c>
@@ -23953,7 +23953,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>609</v>
       </c>
@@ -23991,7 +23991,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>471</v>
       </c>
@@ -24254,7 +24254,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="108" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>672</v>
       </c>
@@ -24292,7 +24292,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>528</v>
       </c>
@@ -24330,7 +24330,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>610</v>
       </c>
@@ -24368,7 +24368,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>527</v>
       </c>
@@ -34986,7 +34986,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="410" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B410" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35050,7 +35050,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="412" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="412" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="B412" s="43" t="s">
         <v>1355</v>
       </c>
@@ -35862,7 +35862,7 @@
   <autoFilter ref="A1:N437">
     <filterColumn colId="2">
       <filters>
-        <filter val="351-00-T2"/>
+        <filter val="251-00-T2"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -36169,18 +36169,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36203,14 +36203,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56C8FBF-B3B9-432D-A40E-5376C0AE01AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02A70B78-95E3-4533-A5C0-CF911D481E23}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="42bcbbcd-ff49-4650-acba-18717079aec5"/>
@@ -36225,4 +36217,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56C8FBF-B3B9-432D-A40E-5376C0AE01AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>